<commit_message>
Added a view to the XLS showing exactly what we are voting next as opposed to the whole issue list
</commit_message>
<xml_diff>
--- a/docs/dds-psm-cxx-ftf-votes.xlsx
+++ b/docs/dds-psm-cxx-ftf-votes.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="260" windowWidth="21780" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="5300" yWindow="180" windowWidth="21780" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Voting Now" sheetId="2" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Issue #</t>
   </si>
@@ -143,9 +144,6 @@
   </si>
   <si>
     <t>RadarTrack uses anonymous types</t>
-  </si>
-  <si>
-    <t>Defer</t>
   </si>
   <si>
     <t xml:space="preserve">Stdlib class for Optional support </t>
@@ -290,8 +288,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,15 +341,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -678,11 +680,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -725,13 +727,13 @@
     </row>
     <row r="3" spans="2:11">
       <c r="B3" s="10">
-        <v>15965</v>
+        <v>16308</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E3" s="3"/>
       <c r="G3" s="10"/>
@@ -744,13 +746,13 @@
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="10">
-        <v>15976</v>
+        <v>16338</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E4" s="3"/>
       <c r="G4" s="10"/>
@@ -763,13 +765,13 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="10">
-        <v>16261</v>
+        <v>16339</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="10"/>
@@ -782,13 +784,13 @@
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="10">
-        <v>16269</v>
+        <v>16374</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="E6" s="3"/>
       <c r="G6" s="10"/>
@@ -799,15 +801,15 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" ht="30">
       <c r="B7" s="10">
-        <v>16308</v>
+        <v>16411</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="E7" s="3"/>
       <c r="G7" s="10"/>
@@ -820,10 +822,10 @@
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="10">
-        <v>16338</v>
+        <v>16562</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>15</v>
@@ -839,10 +841,10 @@
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="10">
-        <v>16339</v>
+        <v>16563</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>15</v>
@@ -856,6 +858,174 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="11"/>
+    <col min="3" max="3" width="35.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="10">
+        <v>15965</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="10">
+        <v>15976</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="10">
+        <v>16261</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="10">
+        <v>16269</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="10">
+        <v>16308</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="10">
+        <v>16338</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="10">
+        <v>16339</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
     <row r="10" spans="2:11">
       <c r="B10" s="10">
         <v>16340</v>
@@ -863,14 +1033,10 @@
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="3"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -882,14 +1048,10 @@
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="3"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -906,9 +1068,7 @@
       </c>
       <c r="E12" s="3"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -920,14 +1080,10 @@
       <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="D13" s="13"/>
       <c r="E13" s="3"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -939,14 +1095,10 @@
       <c r="C14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="D14" s="13"/>
       <c r="E14" s="3"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -958,14 +1110,10 @@
       <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="D15" s="13"/>
       <c r="E15" s="3"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -977,14 +1125,10 @@
       <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="D16" s="13"/>
       <c r="E16" s="3"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -996,12 +1140,10 @@
       <c r="C17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="3"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -1018,9 +1160,7 @@
       </c>
       <c r="E18" s="3"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -1037,9 +1177,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -1056,9 +1194,7 @@
       </c>
       <c r="E20" s="3"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -1068,16 +1204,12 @@
         <v>16564</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="12" t="s">
         <v>30</v>
       </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="3"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -1087,16 +1219,12 @@
         <v>16565</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="3"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>

</xml_diff>